<commit_message>
Updated FIN model - 2025-08-25 18:15
</commit_message>
<xml_diff>
--- a/VerveStacks_FIN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_FIN/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FIN\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14E4573D-7CF3-45AE-BAC2-5B7FB39A973A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4992C096-5EBF-4482-A5DF-12C3FA7828EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -685,16 +685,22 @@
     <t>wind resource -- CF class won-FIN_47 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-FIN_39_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-FIN_39 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-FIN_39_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-FIN_39 -- cost class 1</t>
   </si>
   <si>
-    <t>e_won-FIN_39_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-FIN_39 -- cost class 4</t>
+    <t>e_won-FIN_39_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-FIN_39 -- cost class 3</t>
   </si>
   <si>
     <t>e_won-FIN_39_c5</t>
@@ -703,12 +709,6 @@
     <t>wind resource -- CF class won-FIN_39 -- cost class 5</t>
   </si>
   <si>
-    <t>e_won-FIN_39_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-FIN_39 -- cost class 3</t>
-  </si>
-  <si>
     <t>e_won-FIN_39_c2</t>
   </si>
   <si>
@@ -787,16 +787,16 @@
     <t>wind resource -- CF class won-FIN_33 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-FIN_33_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-FIN_33 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_won-FIN_33_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-FIN_33 -- cost class 2</t>
-  </si>
-  <si>
-    <t>e_won-FIN_33_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-FIN_33 -- cost class 3</t>
   </si>
   <si>
     <t>e_won-FIN_32_c2</t>
@@ -2265,7 +2265,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40965F53-14C3-513B-2D0F-C8ABD41C6B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86262BF2-ECC4-0A78-6049-BDE153AB95BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2320,7 +2320,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD80C9E3-A589-9261-009C-390ED0D1158B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E38DFF19-289D-C3C0-AB60-8976947B16EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2375,7 +2375,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D8AE7D7-87C0-1B96-1D05-0871789E756B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D75E5FD-827F-D0DB-30DB-B5580F0FE0C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2430,7 +2430,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5496E55-0C5B-26C3-51AF-8B5F3473757C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B5F9B59-CB4F-919C-B81C-995ABE7792EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6360,7 +6360,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC1CB2D-FD9F-4ECD-A000-F7DDB8CB72AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B9D5E1-6147-454B-90F5-388DFE075F00}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6494,7 +6494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522EA642-693E-4240-8E1C-72FD2CF9528F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC73EC1-A1C9-48C1-8AD0-10D03A829218}">
   <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6647,16 +6647,16 @@
         <v>339</v>
       </c>
       <c r="M5" s="163">
-        <v>2.2214999999999998</v>
+        <v>2.5327500000000001</v>
       </c>
       <c r="N5" s="163">
         <v>0.39200000000000002</v>
       </c>
       <c r="O5" s="164">
-        <v>36.31780459989978</v>
+        <v>50.20165214980905</v>
       </c>
       <c r="P5" s="159">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -6688,16 +6688,16 @@
         <v>339</v>
       </c>
       <c r="M6" s="161">
-        <v>2.5327500000000001</v>
+        <v>2.2214999999999998</v>
       </c>
       <c r="N6" s="161">
         <v>0.39200000000000002</v>
       </c>
       <c r="O6" s="162">
-        <v>50.20165214980905</v>
+        <v>36.31780459989978</v>
       </c>
       <c r="P6" s="158">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -6729,16 +6729,16 @@
         <v>339</v>
       </c>
       <c r="M7" s="163">
-        <v>1.8480000000000001</v>
+        <v>3.8610000000000002</v>
       </c>
       <c r="N7" s="163">
         <v>0.38700000000000001</v>
       </c>
       <c r="O7" s="164">
-        <v>53.921482909352299</v>
+        <v>40.945076375777049</v>
       </c>
       <c r="P7" s="159">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -6770,16 +6770,16 @@
         <v>339</v>
       </c>
       <c r="M8" s="161">
-        <v>3.8610000000000002</v>
+        <v>1.8480000000000001</v>
       </c>
       <c r="N8" s="161">
         <v>0.38700000000000001</v>
       </c>
       <c r="O8" s="162">
-        <v>40.945076375777049</v>
+        <v>53.921482909352299</v>
       </c>
       <c r="P8" s="158">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -7344,16 +7344,16 @@
         <v>339</v>
       </c>
       <c r="M22" s="161">
-        <v>0.94499999999999995</v>
+        <v>1.28925</v>
       </c>
       <c r="N22" s="161">
         <v>0.32600000000000001</v>
       </c>
       <c r="O22" s="162">
-        <v>29.596245817095351</v>
+        <v>36.402053439599889</v>
       </c>
       <c r="P22" s="158">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:16">
@@ -7385,16 +7385,16 @@
         <v>339</v>
       </c>
       <c r="M23" s="163">
-        <v>1.28925</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="N23" s="163">
         <v>0.32600000000000001</v>
       </c>
       <c r="O23" s="164">
-        <v>36.402053439599889</v>
+        <v>29.596245817095351</v>
       </c>
       <c r="P23" s="159">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -9785,7 +9785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9EDF50-7340-4CD1-95D6-3B8AAC92485E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366D2E02-EACB-4DD2-A22C-88EF20A8F058}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>